<commit_message>
New Sava Template Upload
</commit_message>
<xml_diff>
--- a/Authentication.WEB/ExcelSavaTemplate/SAVA_Policy_Template_Final.xlsx
+++ b/Authentication.WEB/ExcelSavaTemplate/SAVA_Policy_Template_Final.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Miteski\Desktop\Test sava policy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Miteski\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,30 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Број на полиса</t>
   </si>
   <si>
-    <t>МБР осигуреник</t>
+    <t>ЕМБГ</t>
   </si>
   <si>
-    <t xml:space="preserve">МБР </t>
+    <t>Датум на креирање</t>
   </si>
   <si>
     <t>Датум на истекување</t>
   </si>
   <si>
     <t>Премија</t>
-  </si>
-  <si>
-    <t>0604993489002</t>
-  </si>
-  <si>
-    <t>12/11/2017</t>
-  </si>
-  <si>
-    <t>0607993450040</t>
   </si>
 </sst>
 </file>
@@ -83,9 +74,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,19 +390,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -432,23 +420,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>123050</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>2500</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>